<commit_message>
[Doc] Done with datasheet research.
Resolves #1.
</commit_message>
<xml_diff>
--- a/datasheets/OBCI_Cyton_BOM.xlsx
+++ b/datasheets/OBCI_Cyton_BOM.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\eleggo-hardware\datasheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\eleggo-hardware\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1F7F9E-9567-4DD5-AD2C-403699BBD3E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19344" windowHeight="9168"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="135">
   <si>
     <t>OBCI_V3_C</t>
   </si>
@@ -362,13 +361,76 @@
   </si>
   <si>
     <t>https://store.comet.bg/Catalogue/Product/48428/</t>
+  </si>
+  <si>
+    <t>Datasheet</t>
+  </si>
+  <si>
+    <t>✓</t>
+  </si>
+  <si>
+    <t>https://store.comet.bg/Catalogue/Product/51527/</t>
+  </si>
+  <si>
+    <t>https://store.comet.bg/Catalogue/Product/16603/</t>
+  </si>
+  <si>
+    <t>https://store.comet.bg/Catalogue/Product/49230/</t>
+  </si>
+  <si>
+    <t>https://store.comet.bg/Catalogue/Product/48671/</t>
+  </si>
+  <si>
+    <t>https://store.comet.bg/Catalogue/Product/50861/</t>
+  </si>
+  <si>
+    <t>https://store.comet.bg/Catalogue/Product/35141/</t>
+  </si>
+  <si>
+    <t>https://store.comet.bg/Catalogue/Product/35161/</t>
+  </si>
+  <si>
+    <t>https://store.comet.bg/Catalogue/Product/35159/</t>
+  </si>
+  <si>
+    <t>https://store.comet.bg/Catalogue/Product/48303/</t>
+  </si>
+  <si>
+    <t>https://store.comet.bg/Catalogue/Product/5163393/</t>
+  </si>
+  <si>
+    <t>https://store.comet.bg/Catalogue/Product/49964/</t>
+  </si>
+  <si>
+    <t>https://store.comet.bg/Catalogue/Product/20857/</t>
+  </si>
+  <si>
+    <t>https://store.comet.bg/Catalogue/Product/51644/</t>
+  </si>
+  <si>
+    <t>https://store.comet.bg/Catalogue/Product/91009/</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>ESP-07</t>
+  </si>
+  <si>
+    <t>https://store.comet.bg/CatalogueFarnell/Product/1936100/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -385,6 +447,38 @@
       <color theme="10"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -400,7 +494,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -423,16 +517,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -455,8 +593,55 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1645,30 +1830,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IR35"/>
+  <dimension ref="A1:IR37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="H3:I14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6" defaultRowHeight="12.9" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.69921875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.69140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="26" style="1" customWidth="1"/>
     <col min="3" max="3" width="3" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.09765625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="35.09765625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="28.8984375" style="1" customWidth="1"/>
-    <col min="9" max="252" width="6" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.07421875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.07421875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.4609375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="35.07421875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="28.921875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.4609375" style="8" customWidth="1"/>
+    <col min="10" max="252" width="6" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1679,8 +1865,9 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="6"/>
-    </row>
-    <row r="2" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I1" s="9"/>
+    </row>
+    <row r="2" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1705,8 +1892,11 @@
       <c r="H2" s="7" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I2" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <f>ROW(A3)-2</f>
         <v>1</v>
@@ -1729,11 +1919,14 @@
       <c r="G3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="12" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I3" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <f t="shared" ref="A4:A35" si="0">ROW(A4)-2</f>
         <v>2</v>
@@ -1756,11 +1949,14 @@
       <c r="G4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="12" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I4" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1783,11 +1979,14 @@
       <c r="G5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="12" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I5" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1810,11 +2009,14 @@
       <c r="G6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="12" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I6" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1837,11 +2039,14 @@
       <c r="G7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="12" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I7" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1864,11 +2069,14 @@
       <c r="G8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="12" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I8" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1891,11 +2099,14 @@
       <c r="G9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="12" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I9" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1918,11 +2129,14 @@
       <c r="G10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="12" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I10" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1945,11 +2159,14 @@
       <c r="G11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="12" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I11" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1972,11 +2189,14 @@
       <c r="G12" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="12" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I12" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1997,11 +2217,14 @@
       <c r="G13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="12" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I13" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2022,11 +2245,14 @@
       <c r="G14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="12" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I14" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2047,9 +2273,11 @@
       <c r="G15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I15" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2070,9 +2298,14 @@
       <c r="G16" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H16" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2093,9 +2326,14 @@
       <c r="G17" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H17" s="6"/>
-    </row>
-    <row r="18" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H17" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2116,9 +2354,14 @@
       <c r="G18" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H18" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2139,9 +2382,14 @@
       <c r="G19" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H19" s="6"/>
-    </row>
-    <row r="20" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H19" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2162,9 +2410,12 @@
       <c r="G20" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H20" s="6"/>
-    </row>
-    <row r="21" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H20" s="12"/>
+      <c r="I20" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2185,9 +2436,12 @@
       <c r="G21" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H21" s="13"/>
+      <c r="I21" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2210,9 +2464,14 @@
       <c r="G22" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H22" s="6"/>
-    </row>
-    <row r="23" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H22" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2233,9 +2492,14 @@
       <c r="G23" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H23" s="6"/>
-    </row>
-    <row r="24" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H23" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2256,9 +2520,14 @@
       <c r="G24" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H24" s="6"/>
-    </row>
-    <row r="25" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H24" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2279,9 +2548,14 @@
       <c r="G25" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H25" s="6"/>
-    </row>
-    <row r="26" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H25" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2304,9 +2578,12 @@
       <c r="G26" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="H26" s="6"/>
-    </row>
-    <row r="27" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H26" s="12"/>
+      <c r="I26" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2329,9 +2606,14 @@
       <c r="G27" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="H27" s="6"/>
-    </row>
-    <row r="28" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H27" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2354,9 +2636,14 @@
       <c r="G28" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="H28" s="6"/>
-    </row>
-    <row r="29" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H28" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2379,9 +2666,14 @@
       <c r="G29" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="H29" s="6"/>
-    </row>
-    <row r="30" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H29" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2404,9 +2696,14 @@
       <c r="G30" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H30" s="6"/>
-    </row>
-    <row r="31" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H30" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2427,9 +2724,12 @@
       <c r="G31" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="H31" s="6"/>
-    </row>
-    <row r="32" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H31" s="12"/>
+      <c r="I31" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2450,9 +2750,11 @@
       <c r="G32" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="H32" s="6"/>
-    </row>
-    <row r="33" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I32" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2473,9 +2775,14 @@
       <c r="G33" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="H33" s="6"/>
-    </row>
-    <row r="34" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H33" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2496,48 +2803,89 @@
       <c r="G34" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="H34" s="7"/>
-    </row>
-    <row r="35" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="4">
+      <c r="H34" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="14">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="14">
         <v>1</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="3" t="s">
+      <c r="E35" s="16"/>
+      <c r="F35" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="G35" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="H35" s="6"/>
+      <c r="H35" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="I35" s="18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="E36" s="19"/>
+      <c r="F36" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="H36" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="I36" s="18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G37" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1" xr:uid="{FEB5E9E2-259F-4322-B690-D2547E90FE58}"/>
-    <hyperlink ref="H14" r:id="rId2" xr:uid="{BE76AE93-7CC7-414D-96F6-D6FD21342C37}"/>
-    <hyperlink ref="H13" r:id="rId3" xr:uid="{EA8D4019-B922-44B7-A5D5-309FCA83BE74}"/>
-    <hyperlink ref="H12" r:id="rId4" xr:uid="{DE2EA0BA-0440-4BFA-8EC5-F5197B4516E9}"/>
-    <hyperlink ref="H11" r:id="rId5" xr:uid="{13836BDC-2B0F-4140-90FD-303EFE6D506B}"/>
-    <hyperlink ref="H10" r:id="rId6" xr:uid="{6B18D8F2-969D-4013-B6D9-35747F7D35F5}"/>
-    <hyperlink ref="H9" r:id="rId7" xr:uid="{6CA79503-AFAA-46E9-AF70-CD686C243590}"/>
-    <hyperlink ref="H8" r:id="rId8" xr:uid="{40E6E6CD-83B2-4DEE-B374-93B2CEF5B567}"/>
-    <hyperlink ref="H7" r:id="rId9" xr:uid="{A00F979A-0D9D-41B2-BB7B-4E684CE7D440}"/>
-    <hyperlink ref="H6" r:id="rId10" xr:uid="{B1962D36-166F-4CC6-BD8A-8ACCDF68EB33}"/>
-    <hyperlink ref="H5" r:id="rId11" xr:uid="{AA4535B9-AB4E-4697-8055-B96EFF9567F6}"/>
-    <hyperlink ref="H4" r:id="rId12" xr:uid="{A20CB05F-79E5-45D1-B4CB-FE7E072E21CB}"/>
+    <hyperlink ref="H3" r:id="rId1"/>
+    <hyperlink ref="H14" r:id="rId2"/>
+    <hyperlink ref="H13" r:id="rId3"/>
+    <hyperlink ref="H12" r:id="rId4"/>
+    <hyperlink ref="H11" r:id="rId5"/>
+    <hyperlink ref="H10" r:id="rId6"/>
+    <hyperlink ref="H9" r:id="rId7"/>
+    <hyperlink ref="H8" r:id="rId8"/>
+    <hyperlink ref="H7" r:id="rId9"/>
+    <hyperlink ref="H6" r:id="rId10"/>
+    <hyperlink ref="H5" r:id="rId11"/>
+    <hyperlink ref="H4" r:id="rId12"/>
+    <hyperlink ref="H17" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>

</xml_diff>